<commit_message>
add in completeness hceck, range violation check and rushing participants check
</commit_message>
<xml_diff>
--- a/information/2025-10-28_Item_Information_Adults.xlsx
+++ b/information/2025-10-28_Item_Information_Adults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Wilken Arbeitsordner\Clinical_Backbone_RU5389\information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21391553-6B83-4B51-97F7-98EE7E6290C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E777E77-D197-40E5-9123-2F800D077BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31530" yWindow="2865" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2920" uniqueCount="1400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2927" uniqueCount="1401">
   <si>
     <t>Item</t>
   </si>
@@ -4225,6 +4225,9 @@
   </si>
   <si>
     <t>TICS</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -4630,7 +4633,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4668,6 +4671,9 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3" t="s">
+        <v>1400</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -4688,11 +4694,17 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
+      <c r="B7" t="s">
+        <v>1400</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
+      <c r="B8" t="s">
+        <v>1400</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -4703,20 +4715,32 @@
       <c r="A10" t="s">
         <v>12</v>
       </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
implemented descriptive data analysis v0.1
</commit_message>
<xml_diff>
--- a/information/2025-10-28_Item_Information_Adults.xlsx
+++ b/information/2025-10-28_Item_Information_Adults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Wilken Arbeitsordner\Clinical_Backbone_RU5389\information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E777E77-D197-40E5-9123-2F800D077BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F9F93C-892A-4380-ABC0-BCEA280358F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31530" yWindow="2865" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4632,8 +4632,8 @@
   <dimension ref="A1:E1325"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <pane ySplit="1" topLeftCell="A1130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4724,7 +4724,7 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
read.csv issue fix, no more renaming psytoolkit output
weird bugs appeared that required hours of fixing
improved robustness of code in many places
hopefully fixed that no more empty cogntiive tests are in the output
removed need to rename psytoolkit download
some surgical indivudal vpid fixes
currently still running into issues because of type mismatches between questionnaires...
</commit_message>
<xml_diff>
--- a/information/2025-10-28_Item_Information_Adults.xlsx
+++ b/information/2025-10-28_Item_Information_Adults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Wilken Arbeitsordner\Clinical_Backbone_RU5389\information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F9F93C-892A-4380-ABC0-BCEA280358F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FE75C0-8A5F-4453-B948-DA1342B68479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31530" yWindow="2865" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2927" uniqueCount="1401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2931" uniqueCount="1405">
   <si>
     <t>Item</t>
   </si>
@@ -4228,6 +4228,18 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>HiTOP-Subfactor</t>
+  </si>
+  <si>
+    <t>HiTOP-Spectrum</t>
+  </si>
+  <si>
+    <t>RDoC System</t>
+  </si>
+  <si>
+    <t>RDoC Construct</t>
   </si>
 </sst>
 </file>
@@ -4259,7 +4271,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -4282,13 +4294,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -4629,11 +4655,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1325"/>
+  <dimension ref="A1:I1325"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1130" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4642,10 +4668,11 @@
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4658,16 +4685,28 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>1402</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1401</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1403</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1404</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4675,22 +4714,22 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -4698,7 +4737,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -4706,12 +4745,12 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -4719,7 +4758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4727,7 +4766,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -4735,7 +4774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -4743,17 +4782,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -6532,7 +6571,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>147</v>
       </c>
@@ -6546,7 +6585,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>148</v>
       </c>
@@ -6560,7 +6599,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>149</v>
       </c>
@@ -6574,7 +6613,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>150</v>
       </c>
@@ -6588,7 +6627,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>151</v>
       </c>
@@ -6602,7 +6641,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>152</v>
       </c>
@@ -6616,7 +6655,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>153</v>
       </c>
@@ -6630,7 +6669,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>154</v>
       </c>
@@ -6644,7 +6683,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>155</v>
       </c>
@@ -6658,7 +6697,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>156</v>
       </c>
@@ -6672,7 +6711,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>157</v>
       </c>
@@ -6686,7 +6725,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>158</v>
       </c>
@@ -6700,7 +6739,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>159</v>
       </c>
@@ -6711,7 +6750,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>160</v>
       </c>
@@ -6722,7 +6761,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>161</v>
       </c>
@@ -6732,11 +6771,11 @@
       <c r="C159" t="s">
         <v>1381</v>
       </c>
-      <c r="E159" t="s">
+      <c r="I159" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>162</v>
       </c>
@@ -6746,11 +6785,11 @@
       <c r="C160" t="s">
         <v>1381</v>
       </c>
-      <c r="E160" t="s">
+      <c r="I160" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>163</v>
       </c>
@@ -6760,11 +6799,11 @@
       <c r="C161" t="s">
         <v>1381</v>
       </c>
-      <c r="E161" t="s">
+      <c r="I161" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>164</v>
       </c>
@@ -6774,11 +6813,11 @@
       <c r="C162" t="s">
         <v>1381</v>
       </c>
-      <c r="E162" t="s">
+      <c r="I162" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>165</v>
       </c>
@@ -6788,11 +6827,11 @@
       <c r="C163" t="s">
         <v>1381</v>
       </c>
-      <c r="E163" t="s">
+      <c r="I163" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>166</v>
       </c>
@@ -6802,11 +6841,11 @@
       <c r="C164" t="s">
         <v>1381</v>
       </c>
-      <c r="E164" t="s">
+      <c r="I164" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>167</v>
       </c>
@@ -6817,7 +6856,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>168</v>
       </c>
@@ -6828,7 +6867,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>169</v>
       </c>
@@ -6839,7 +6878,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>170</v>
       </c>
@@ -6850,7 +6889,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>171</v>
       </c>
@@ -6861,7 +6900,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>172</v>
       </c>
@@ -6872,7 +6911,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>173</v>
       </c>
@@ -6883,7 +6922,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>174</v>
       </c>
@@ -6894,7 +6933,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>175</v>
       </c>
@@ -6905,7 +6944,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>176</v>
       </c>
@@ -6916,7 +6955,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>177</v>
       </c>
@@ -6927,7 +6966,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>178</v>
       </c>
@@ -7114,7 +7153,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>195</v>
       </c>
@@ -7125,7 +7164,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>196</v>
       </c>
@@ -7136,7 +7175,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>197</v>
       </c>
@@ -7147,7 +7186,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>198</v>
       </c>
@@ -7158,7 +7197,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>199</v>
       </c>
@@ -7169,7 +7208,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>200</v>
       </c>
@@ -7180,7 +7219,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>201</v>
       </c>
@@ -7191,7 +7230,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>202</v>
       </c>
@@ -7202,7 +7241,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>203</v>
       </c>
@@ -7215,11 +7254,11 @@
       <c r="D201" t="s">
         <v>1333</v>
       </c>
-      <c r="E201" t="s">
+      <c r="I201" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>204</v>
       </c>
@@ -7233,7 +7272,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>205</v>
       </c>
@@ -7247,7 +7286,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>206</v>
       </c>
@@ -7261,7 +7300,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>207</v>
       </c>
@@ -7272,7 +7311,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>208</v>
       </c>
@@ -7286,7 +7325,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>209</v>
       </c>
@@ -7300,7 +7339,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>210</v>
       </c>
@@ -7314,7 +7353,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>211</v>
       </c>
@@ -7328,7 +7367,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>212</v>
       </c>
@@ -7339,7 +7378,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>213</v>
       </c>
@@ -7353,7 +7392,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>214</v>
       </c>
@@ -7367,7 +7406,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>215</v>
       </c>
@@ -7381,7 +7420,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>216</v>
       </c>
@@ -7395,7 +7434,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>217</v>
       </c>
@@ -7409,7 +7448,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>218</v>
       </c>
@@ -7420,7 +7459,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>219</v>
       </c>
@@ -7434,7 +7473,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>220</v>
       </c>
@@ -7448,7 +7487,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>221</v>
       </c>
@@ -7462,7 +7501,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>222</v>
       </c>
@@ -7476,7 +7515,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>223</v>
       </c>
@@ -7489,11 +7528,11 @@
       <c r="D221" t="s">
         <v>1333</v>
       </c>
-      <c r="E221" t="s">
+      <c r="I221" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>224</v>
       </c>
@@ -7507,7 +7546,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>225</v>
       </c>
@@ -7521,7 +7560,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>226</v>
       </c>
@@ -7708,7 +7747,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>243</v>
       </c>
@@ -7719,7 +7758,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>244</v>
       </c>
@@ -7730,7 +7769,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>245</v>
       </c>
@@ -7741,7 +7780,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>246</v>
       </c>
@@ -7752,7 +7791,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>247</v>
       </c>
@@ -7763,7 +7802,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>248</v>
       </c>
@@ -7774,7 +7813,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>249</v>
       </c>
@@ -7785,7 +7824,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>250</v>
       </c>
@@ -7796,7 +7835,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>251</v>
       </c>
@@ -7807,7 +7846,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>252</v>
       </c>
@@ -7818,7 +7857,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>253</v>
       </c>
@@ -7828,11 +7867,11 @@
       <c r="D251" t="s">
         <v>1390</v>
       </c>
-      <c r="E251" t="s">
+      <c r="I251" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>254</v>
       </c>
@@ -7843,7 +7882,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>255</v>
       </c>
@@ -7854,7 +7893,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>256</v>
       </c>
@@ -7865,7 +7904,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>257</v>
       </c>
@@ -7876,7 +7915,7 @@
         <v>1390</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>258</v>
       </c>
@@ -8036,7 +8075,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>275</v>
       </c>
@@ -8046,11 +8085,11 @@
       <c r="D273" t="s">
         <v>1370</v>
       </c>
-      <c r="E273" t="s">
+      <c r="I273" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>276</v>
       </c>
@@ -8061,7 +8100,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>277</v>
       </c>
@@ -8072,7 +8111,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>278</v>
       </c>
@@ -8082,11 +8121,11 @@
       <c r="D276" t="s">
         <v>1372</v>
       </c>
-      <c r="E276" t="s">
+      <c r="I276" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>279</v>
       </c>
@@ -8097,7 +8136,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>280</v>
       </c>
@@ -8107,11 +8146,11 @@
       <c r="D278" t="s">
         <v>1372</v>
       </c>
-      <c r="E278" t="s">
+      <c r="I278" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>281</v>
       </c>
@@ -8122,7 +8161,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>282</v>
       </c>
@@ -8133,7 +8172,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>283</v>
       </c>
@@ -8144,7 +8183,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>284</v>
       </c>
@@ -8155,7 +8194,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>285</v>
       </c>
@@ -8166,7 +8205,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>286</v>
       </c>
@@ -8176,11 +8215,11 @@
       <c r="D284" t="s">
         <v>1372</v>
       </c>
-      <c r="E284" t="s">
+      <c r="I284" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>287</v>
       </c>
@@ -8191,7 +8230,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>288</v>
       </c>
@@ -8202,7 +8241,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>289</v>
       </c>
@@ -8213,7 +8252,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>290</v>
       </c>
@@ -8224,7 +8263,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>291</v>
       </c>
@@ -8235,7 +8274,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>292</v>
       </c>
@@ -8245,11 +8284,11 @@
       <c r="D290" t="s">
         <v>1372</v>
       </c>
-      <c r="E290" t="s">
+      <c r="I290" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>293</v>
       </c>
@@ -8260,7 +8299,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>294</v>
       </c>
@@ -8271,7 +8310,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>295</v>
       </c>
@@ -8282,7 +8321,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>296</v>
       </c>
@@ -8293,7 +8332,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>297</v>
       </c>
@@ -8304,7 +8343,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>298</v>
       </c>
@@ -8315,7 +8354,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>299</v>
       </c>
@@ -8325,11 +8364,11 @@
       <c r="D297" t="s">
         <v>1370</v>
       </c>
-      <c r="E297" t="s">
+      <c r="I297" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>300</v>
       </c>
@@ -8340,7 +8379,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>301</v>
       </c>
@@ -8350,186 +8389,186 @@
       <c r="D299" t="s">
         <v>1372</v>
       </c>
-      <c r="E299" t="s">
+      <c r="I299" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>303</v>
       </c>
       <c r="B301" t="s">
         <v>1338</v>
       </c>
-      <c r="E301" t="s">
+      <c r="I301" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>304</v>
       </c>
       <c r="B302" t="s">
         <v>1338</v>
       </c>
-      <c r="E302" t="s">
+      <c r="I302" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>305</v>
       </c>
       <c r="B303" t="s">
         <v>1338</v>
       </c>
-      <c r="E303" t="s">
+      <c r="I303" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>307</v>
       </c>
       <c r="B305" t="s">
         <v>1338</v>
       </c>
-      <c r="E305" t="s">
+      <c r="I305" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>308</v>
       </c>
       <c r="B306" t="s">
         <v>1338</v>
       </c>
-      <c r="E306" t="s">
+      <c r="I306" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>309</v>
       </c>
       <c r="B307" t="s">
         <v>1338</v>
       </c>
-      <c r="E307" t="s">
+      <c r="I307" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>310</v>
       </c>
       <c r="B308" t="s">
         <v>1338</v>
       </c>
-      <c r="E308" t="s">
+      <c r="I308" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>311</v>
       </c>
       <c r="B309" t="s">
         <v>1338</v>
       </c>
-      <c r="E309" t="s">
+      <c r="I309" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>312</v>
       </c>
       <c r="B310" t="s">
         <v>1338</v>
       </c>
-      <c r="E310" t="s">
+      <c r="I310" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>313</v>
       </c>
       <c r="B311" t="s">
         <v>1338</v>
       </c>
-      <c r="E311" t="s">
+      <c r="I311" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>314</v>
       </c>
       <c r="B312" t="s">
         <v>1338</v>
       </c>
-      <c r="E312" t="s">
+      <c r="I312" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>315</v>
       </c>
       <c r="B313" t="s">
         <v>1338</v>
       </c>
-      <c r="E313" t="s">
+      <c r="I313" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>316</v>
       </c>
       <c r="B314" t="s">
         <v>1338</v>
       </c>
-      <c r="E314" t="s">
+      <c r="I314" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>317</v>
       </c>
       <c r="B315" t="s">
         <v>1338</v>
       </c>
-      <c r="E315" t="s">
+      <c r="I315" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>318</v>
       </c>
       <c r="B316" t="s">
         <v>1338</v>
       </c>
-      <c r="E316" t="s">
+      <c r="I316" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>319</v>
       </c>
@@ -8537,7 +8576,7 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>320</v>
       </c>
@@ -8545,7 +8584,7 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>321</v>
       </c>
@@ -8553,7 +8592,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>322</v>
       </c>

</xml_diff>

<commit_message>
mapping, scoruing and plotting of items imporved
completed hitop mapping of items
added SUQ scoring
fuixed plotting scripts
fixed internal consistency script
recoded some wrongly coded items
added initial draft of factor analysis script
</commit_message>
<xml_diff>
--- a/information/2025-10-28_Item_Information_Adults.xlsx
+++ b/information/2025-10-28_Item_Information_Adults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Wilken Arbeitsordner\Clinical_Backbone_RU5389\information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2D0E4B-3529-4BAD-A785-8A58DD0FF264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32CEE98-2D6C-4A33-986E-CB08C3CC91CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3429" uniqueCount="1428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3569" uniqueCount="1432">
   <si>
     <t>Item</t>
   </si>
@@ -4287,9 +4287,6 @@
     <t>trauma_reactions</t>
   </si>
   <si>
-    <t>spec_phobia_ind</t>
-  </si>
-  <si>
     <t>internaliz-thought_dis</t>
   </si>
   <si>
@@ -4309,6 +4306,21 @@
   </si>
   <si>
     <t>disinh_antisoc_extern</t>
+  </si>
+  <si>
+    <t>eating_pathology</t>
+  </si>
+  <si>
+    <t>well-being</t>
+  </si>
+  <si>
+    <t>fear</t>
+  </si>
+  <si>
+    <t>binge-eating</t>
+  </si>
+  <si>
+    <t>emotionality</t>
   </si>
 </sst>
 </file>
@@ -4727,8 +4739,8 @@
   <dimension ref="A1:K1325"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F199" sqref="F195:F199"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4872,17 +4884,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -4902,10 +4914,13 @@
         <v>1405</v>
       </c>
       <c r="G19" t="s">
+        <v>1427</v>
+      </c>
+      <c r="H19" t="s">
         <v>1339</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -4925,10 +4940,13 @@
         <v>1405</v>
       </c>
       <c r="G20" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H20" t="s">
         <v>1416</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -4945,10 +4963,16 @@
         <v>1408</v>
       </c>
       <c r="F21" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1422</v>
+      </c>
+      <c r="H21" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K21" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -4968,10 +4992,13 @@
         <v>1405</v>
       </c>
       <c r="G22" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H22" t="s">
         <v>1342</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -4991,10 +5018,13 @@
         <v>1405</v>
       </c>
       <c r="G23" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H23" t="s">
         <v>1416</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -5013,11 +5043,11 @@
       <c r="F24" t="s">
         <v>1405</v>
       </c>
-      <c r="H24" t="s">
-        <v>1343</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -5037,10 +5067,13 @@
         <v>1405</v>
       </c>
       <c r="G25" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H25" t="s">
         <v>1344</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -5063,7 +5096,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -5086,7 +5119,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -5103,10 +5136,16 @@
         <v>1408</v>
       </c>
       <c r="F28" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1422</v>
+      </c>
+      <c r="H28" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K28" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -5126,10 +5165,13 @@
         <v>1405</v>
       </c>
       <c r="G29" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H29" t="s">
         <v>1342</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -5148,8 +5190,11 @@
       <c r="F30" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -5169,10 +5214,13 @@
         <v>1405</v>
       </c>
       <c r="G31" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H31" t="s">
         <v>1346</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -5192,10 +5240,13 @@
         <v>1405</v>
       </c>
       <c r="G32" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H32" t="s">
         <v>1419</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -5212,13 +5263,13 @@
         <v>1409</v>
       </c>
       <c r="F33" t="s">
+        <v>1422</v>
+      </c>
+      <c r="H33" t="s">
         <v>1423</v>
       </c>
-      <c r="G33" t="s">
-        <v>1424</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -5238,10 +5289,13 @@
         <v>1405</v>
       </c>
       <c r="G34" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H34" t="s">
         <v>1344</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -5261,10 +5315,13 @@
         <v>1405</v>
       </c>
       <c r="G35" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H35" t="s">
         <v>1342</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -5281,10 +5338,13 @@
         <v>1408</v>
       </c>
       <c r="F36" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1422</v>
+      </c>
+      <c r="H36" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -5304,10 +5364,13 @@
         <v>1405</v>
       </c>
       <c r="G37" t="s">
+        <v>1427</v>
+      </c>
+      <c r="H37" t="s">
         <v>1418</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -5324,13 +5387,13 @@
         <v>1409</v>
       </c>
       <c r="F38" t="s">
+        <v>1422</v>
+      </c>
+      <c r="H38" t="s">
         <v>1423</v>
       </c>
-      <c r="G38" t="s">
-        <v>1420</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -5353,7 +5416,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -5372,8 +5435,14 @@
       <c r="F40" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H40" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -5390,10 +5459,16 @@
         <v>1408</v>
       </c>
       <c r="F41" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1422</v>
+      </c>
+      <c r="H41" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K41" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -5412,8 +5487,14 @@
       <c r="F42" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>1427</v>
+      </c>
+      <c r="H42" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -5432,8 +5513,14 @@
       <c r="F43" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H43" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -5452,8 +5539,14 @@
       <c r="F44" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>1427</v>
+      </c>
+      <c r="H44" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -5470,10 +5563,16 @@
         <v>1408</v>
       </c>
       <c r="F45" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1422</v>
+      </c>
+      <c r="H45" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K45" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -5492,8 +5591,14 @@
       <c r="F46" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H46" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -5512,8 +5617,11 @@
       <c r="F47" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -5532,8 +5640,11 @@
       <c r="F48" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -5556,7 +5667,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -5575,8 +5686,14 @@
       <c r="F50" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H50" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -5595,8 +5712,14 @@
       <c r="F51" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H51" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -5615,8 +5738,14 @@
       <c r="F52" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H52" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -5635,8 +5764,11 @@
       <c r="F53" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>56</v>
       </c>
@@ -5655,8 +5787,14 @@
       <c r="F54" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H54" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>57</v>
       </c>
@@ -5675,8 +5813,14 @@
       <c r="F55" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H55" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>58</v>
       </c>
@@ -5695,8 +5839,14 @@
       <c r="F56" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H56" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -5719,7 +5869,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -5736,13 +5886,13 @@
         <v>1409</v>
       </c>
       <c r="F58" t="s">
+        <v>1422</v>
+      </c>
+      <c r="H58" t="s">
         <v>1423</v>
       </c>
-      <c r="G58" t="s">
-        <v>1424</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -5761,8 +5911,14 @@
       <c r="F59" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H59" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>62</v>
       </c>
@@ -5781,8 +5937,11 @@
       <c r="F60" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G60" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -5801,8 +5960,11 @@
       <c r="F61" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>64</v>
       </c>
@@ -5821,8 +5983,14 @@
       <c r="F62" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H62" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>65</v>
       </c>
@@ -5841,8 +6009,14 @@
       <c r="F63" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H63" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>66</v>
       </c>
@@ -5859,13 +6033,13 @@
         <v>1409</v>
       </c>
       <c r="F64" t="s">
+        <v>1422</v>
+      </c>
+      <c r="H64" t="s">
         <v>1423</v>
       </c>
-      <c r="G64" t="s">
-        <v>1424</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>67</v>
       </c>
@@ -5888,7 +6062,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>68</v>
       </c>
@@ -5907,8 +6081,14 @@
       <c r="F66" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H66" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>69</v>
       </c>
@@ -5925,10 +6105,16 @@
         <v>1408</v>
       </c>
       <c r="F67" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1422</v>
+      </c>
+      <c r="H67" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K67" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -5947,8 +6133,14 @@
       <c r="F68" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G68" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H68" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>71</v>
       </c>
@@ -5967,8 +6159,14 @@
       <c r="F69" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H69" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>72</v>
       </c>
@@ -5985,10 +6183,16 @@
         <v>1408</v>
       </c>
       <c r="F70" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1422</v>
+      </c>
+      <c r="H70" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K70" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>73</v>
       </c>
@@ -6007,8 +6211,11 @@
       <c r="F71" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G71" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>74</v>
       </c>
@@ -6027,8 +6234,11 @@
       <c r="F72" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G72" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>75</v>
       </c>
@@ -6047,8 +6257,14 @@
       <c r="F73" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G73" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H73" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>76</v>
       </c>
@@ -6071,7 +6287,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>77</v>
       </c>
@@ -6090,8 +6306,14 @@
       <c r="F75" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H75" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>78</v>
       </c>
@@ -6108,10 +6330,16 @@
         <v>1408</v>
       </c>
       <c r="F76" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1422</v>
+      </c>
+      <c r="H76" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K76" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>79</v>
       </c>
@@ -6130,8 +6358,14 @@
       <c r="F77" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G77" t="s">
+        <v>1427</v>
+      </c>
+      <c r="H77" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>80</v>
       </c>
@@ -6150,8 +6384,11 @@
       <c r="F78" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G78" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>81</v>
       </c>
@@ -6170,8 +6407,11 @@
       <c r="F79" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G79" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -6190,8 +6430,14 @@
       <c r="F80" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G80" t="s">
+        <v>1427</v>
+      </c>
+      <c r="H80" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>83</v>
       </c>
@@ -6208,10 +6454,16 @@
         <v>1408</v>
       </c>
       <c r="F81" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1422</v>
+      </c>
+      <c r="H81" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K81" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>84</v>
       </c>
@@ -6230,8 +6482,14 @@
       <c r="F82" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G82" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H82" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>85</v>
       </c>
@@ -6251,10 +6509,13 @@
         <v>1405</v>
       </c>
       <c r="G83" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H83" t="s">
         <v>1351</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>86</v>
       </c>
@@ -6268,16 +6529,19 @@
         <v>1352</v>
       </c>
       <c r="E84" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="F84" t="s">
+        <v>1420</v>
+      </c>
+      <c r="G84" t="s">
+        <v>1352</v>
+      </c>
+      <c r="H84" t="s">
         <v>1421</v>
       </c>
-      <c r="G84" t="s">
-        <v>1422</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>87</v>
       </c>
@@ -6297,10 +6561,13 @@
         <v>1405</v>
       </c>
       <c r="G85" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H85" t="s">
         <v>1353</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>88</v>
       </c>
@@ -6319,8 +6586,14 @@
       <c r="F86" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G86" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H86" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>89</v>
       </c>
@@ -6339,8 +6612,14 @@
       <c r="F87" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G87" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H87" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>90</v>
       </c>
@@ -6357,10 +6636,16 @@
         <v>1408</v>
       </c>
       <c r="F88" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1420</v>
+      </c>
+      <c r="G88" t="s">
+        <v>1352</v>
+      </c>
+      <c r="H88" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>91</v>
       </c>
@@ -6377,10 +6662,16 @@
         <v>1408</v>
       </c>
       <c r="F89" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1422</v>
+      </c>
+      <c r="H89" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K89" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>92</v>
       </c>
@@ -6399,8 +6690,14 @@
       <c r="F90" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G90" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H90" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>93</v>
       </c>
@@ -6419,8 +6716,11 @@
       <c r="F91" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G91" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>94</v>
       </c>
@@ -6439,8 +6739,14 @@
       <c r="F92" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G92" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H92" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>95</v>
       </c>
@@ -6459,8 +6765,14 @@
       <c r="F93" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G93" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H93" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>96</v>
       </c>
@@ -6474,16 +6786,19 @@
         <v>1352</v>
       </c>
       <c r="E94" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="F94" t="s">
+        <v>1420</v>
+      </c>
+      <c r="G94" t="s">
+        <v>1352</v>
+      </c>
+      <c r="H94" t="s">
         <v>1421</v>
       </c>
-      <c r="G94" t="s">
-        <v>1422</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>97</v>
       </c>
@@ -6500,10 +6815,16 @@
         <v>1408</v>
       </c>
       <c r="F95" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1422</v>
+      </c>
+      <c r="H95" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K95" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>98</v>
       </c>
@@ -6522,8 +6843,14 @@
       <c r="F96" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G96" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H96" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>99</v>
       </c>
@@ -6542,8 +6869,11 @@
       <c r="F97" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G97" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>100</v>
       </c>
@@ -6562,8 +6892,14 @@
       <c r="F98" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G98" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H98" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>101</v>
       </c>
@@ -6582,8 +6918,14 @@
       <c r="F99" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G99" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H99" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>102</v>
       </c>
@@ -6597,16 +6939,19 @@
         <v>1352</v>
       </c>
       <c r="E100" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="F100" t="s">
+        <v>1420</v>
+      </c>
+      <c r="G100" t="s">
+        <v>1352</v>
+      </c>
+      <c r="H100" t="s">
         <v>1421</v>
       </c>
-      <c r="G100" t="s">
-        <v>1422</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>103</v>
       </c>
@@ -6625,8 +6970,11 @@
       <c r="F101" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G101" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>104</v>
       </c>
@@ -6645,8 +6993,14 @@
       <c r="F102" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G102" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H102" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>105</v>
       </c>
@@ -6665,8 +7019,14 @@
       <c r="F103" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G103" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H103" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>106</v>
       </c>
@@ -6680,16 +7040,19 @@
         <v>1352</v>
       </c>
       <c r="E104" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="F104" t="s">
+        <v>1420</v>
+      </c>
+      <c r="G104" t="s">
+        <v>1352</v>
+      </c>
+      <c r="H104" t="s">
         <v>1421</v>
       </c>
-      <c r="G104" t="s">
-        <v>1422</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>107</v>
       </c>
@@ -6706,10 +7069,16 @@
         <v>1408</v>
       </c>
       <c r="F105" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1422</v>
+      </c>
+      <c r="H105" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K105" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>108</v>
       </c>
@@ -6728,8 +7097,14 @@
       <c r="F106" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G106" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H106" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>109</v>
       </c>
@@ -6748,8 +7123,11 @@
       <c r="F107" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G107" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>110</v>
       </c>
@@ -6768,8 +7146,14 @@
       <c r="F108" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G108" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H108" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>111</v>
       </c>
@@ -6786,10 +7170,16 @@
         <v>1408</v>
       </c>
       <c r="F109" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1422</v>
+      </c>
+      <c r="H109" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K109" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>112</v>
       </c>
@@ -6808,8 +7198,14 @@
       <c r="F110" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G110" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H110" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>113</v>
       </c>
@@ -6828,8 +7224,11 @@
       <c r="F111" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G111" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>114</v>
       </c>
@@ -6848,8 +7247,14 @@
       <c r="F112" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G112" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H112" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>115</v>
       </c>
@@ -6868,8 +7273,14 @@
       <c r="F113" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G113" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H113" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>116</v>
       </c>
@@ -6886,10 +7297,16 @@
         <v>1408</v>
       </c>
       <c r="F114" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1422</v>
+      </c>
+      <c r="H114" t="s">
+        <v>1428</v>
+      </c>
+      <c r="K114" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>117</v>
       </c>
@@ -6908,8 +7325,14 @@
       <c r="F115" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G115" t="s">
+        <v>1429</v>
+      </c>
+      <c r="H115" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>118</v>
       </c>
@@ -6926,13 +7349,13 @@
         <v>1409</v>
       </c>
       <c r="F116" t="s">
+        <v>1422</v>
+      </c>
+      <c r="H116" t="s">
         <v>1423</v>
       </c>
-      <c r="G116" t="s">
-        <v>1424</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>119</v>
       </c>
@@ -6952,7 +7375,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>120</v>
       </c>
@@ -6972,7 +7395,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>121</v>
       </c>
@@ -6992,7 +7415,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>122</v>
       </c>
@@ -7012,7 +7435,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>123</v>
       </c>
@@ -7032,7 +7455,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>124</v>
       </c>
@@ -7052,7 +7475,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>125</v>
       </c>
@@ -7072,7 +7495,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>126</v>
       </c>
@@ -7092,7 +7515,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>127</v>
       </c>
@@ -7112,7 +7535,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>128</v>
       </c>
@@ -7132,7 +7555,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>129</v>
       </c>
@@ -7152,7 +7575,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>130</v>
       </c>
@@ -8414,10 +8837,10 @@
         <v>1412</v>
       </c>
       <c r="F194" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="G194" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.25">
@@ -8434,10 +8857,10 @@
         <v>1412</v>
       </c>
       <c r="F195" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="G195" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.25">
@@ -8454,10 +8877,10 @@
         <v>1412</v>
       </c>
       <c r="F196" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="G196" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.25">
@@ -8474,10 +8897,10 @@
         <v>1412</v>
       </c>
       <c r="F197" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="G197" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.25">
@@ -8494,10 +8917,10 @@
         <v>1412</v>
       </c>
       <c r="F198" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="G198" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
@@ -8514,10 +8937,10 @@
         <v>1412</v>
       </c>
       <c r="F199" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="G199" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.25">
@@ -9691,6 +10114,9 @@
       <c r="I281" t="s">
         <v>1414</v>
       </c>
+      <c r="K281" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
@@ -9778,6 +10204,9 @@
       <c r="I287" t="s">
         <v>1414</v>
       </c>
+      <c r="K287" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
@@ -9864,6 +10293,9 @@
       </c>
       <c r="I293" t="s">
         <v>1414</v>
+      </c>
+      <c r="K293" t="s">
+        <v>1376</v>
       </c>
     </row>
     <row r="294" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>